<commit_message>
Update Testing level comparison
</commit_message>
<xml_diff>
--- a/Others/Testing levels comparison.xlsx
+++ b/Others/Testing levels comparison.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\NEW_JOB\QA\ISTQB Foundation 4.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Storage\Study Notes\study-notes\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Levels" sheetId="1" r:id="rId1"/>
-    <sheet name="Planning" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="SDLC" sheetId="5" r:id="rId2"/>
+    <sheet name="Planning" sheetId="2" r:id="rId3"/>
+    <sheet name="Static vs Dynamic" sheetId="3" r:id="rId4"/>
+    <sheet name="Test order" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="229">
   <si>
     <t>Test Level</t>
   </si>
@@ -692,39 +694,1605 @@
 After build / deployment</t>
   </si>
   <si>
-    <t>Early in SDLQ
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Cheaper - defect found early</t>
+  </si>
+  <si>
+    <t>Expensive - Defects found late</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Early in SDLQ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Shift-left
 (When requirements, designs are ready)</t>
+    </r>
+  </si>
+  <si>
+    <t>Static Analysis</t>
+  </si>
+  <si>
+    <t>Req / Design Review
+Checklist</t>
   </si>
   <si>
     <t xml:space="preserve">Review
-Static analysis
-Req / Design review checklist
 </t>
   </si>
   <si>
-    <t>- Black-box:
-EP, BVA, Decision Tables, State transition
-- White-box:
-Statement, Branch, Path Coverage
-- Experience-based:
-Error guessing, Exploratory</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Cheaper - defect found early</t>
-  </si>
-  <si>
-    <t>Expensive - Defects found late</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EP (Equivalence Partitioning)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Reduce total test cases by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dividing input data into partitions (valid &amp; invalid sets)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ex: Age 18-65
+Partitions:
+Below valid (≤17)
+Valid (18–65)
+Above valid (≥66)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Decision Tables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Business rules</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>multiple conditions</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Use condition table</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use Case (?)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>End-to-End</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> behavior of User flows</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BVA (Boundary Value Analysis)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Focus on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>edge values / min-max values</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2-point BVA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+[outside-boundary]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3-point BVA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+[out-boundary-in]
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Black-box
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Based on specification</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or external behavior - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">without knowledge of its internal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>structure</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">White-box
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Based on internal structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or logic of component.
+-&gt; Needs to know code, algo &amp; decision path
+-&gt; applied for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unit testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>intergration testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> by Dev or SDETs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Branch</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Goal: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Execute every branch (if-else / true-false)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> at least once
+-&gt; Coverage metrics:
+Decision Coverage = (Executed branches / Total) x 100%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Statement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Goal: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Execute every statement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> at least once
+-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Coverage metrics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Statement Coverage = (Executed statement / Total) x 100%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Path Testing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test every possible path through the program once</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Condition Testing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>boolean conditions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+A = T, B = T
+A = T, B = F
+A = F, B = T
+A = F, B = F
+-&gt; Should use condition table</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Loop Testing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">To find loop boundaries
+- Loop not execute (0 times)
+- Loop executed once
+- Many times
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Infinite loop</t>
+    </r>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>Happy Path</t>
+  </si>
+  <si>
+    <t>Core Logic</t>
+  </si>
+  <si>
+    <t>Basic UI</t>
+  </si>
+  <si>
+    <t>End 2 End</t>
+  </si>
+  <si>
+    <t>Basic Role-based Access</t>
+  </si>
+  <si>
+    <t>Navigation Bar, Layouts
+How to access the feature
+Required Fields
+Confirmation message, toast, popup</t>
+  </si>
+  <si>
+    <t>Business Logic Depth</t>
+  </si>
+  <si>
+    <t>Secondary roles &amp; alternate paths
+Condition logic &amp; calculations
+Edge workflow</t>
+  </si>
+  <si>
+    <t>Integration Points</t>
+  </si>
+  <si>
+    <t>3rd party API calls &amp; error handling</t>
+  </si>
+  <si>
+    <t>Cross-browser Sanity</t>
+  </si>
+  <si>
+    <t>Validate main browserts
+E2E workflow
+Responsive on mobile/tablet</t>
+  </si>
+  <si>
+    <t>Cross-device Sanity</t>
+  </si>
+  <si>
+    <t>iOS, Android</t>
+  </si>
+  <si>
+    <t>Security Basic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance </t>
+  </si>
+  <si>
+    <t>All permutations of workflows
+Low-frequency features (Bulk import/export), reporting, advanved filters</t>
+  </si>
+  <si>
+    <t>Performance &amp; Load test</t>
+  </si>
+  <si>
+    <t>Load/stress testing on APIs and UI endpoints</t>
+  </si>
+  <si>
+    <t>Security Depth</t>
+  </si>
+  <si>
+    <t>Vulnerability scan
+Penetration test
+dependency audit
+Authen/Author bypass attemps</t>
+  </si>
+  <si>
+    <t>Localization &amp; Internationalization</t>
+  </si>
+  <si>
+    <t>Language Packs, currency / date formats RTL text
+Encoding (UTF-8)</t>
+  </si>
+  <si>
+    <t>Cross-Device Long Tail</t>
+  </si>
+  <si>
+    <t>Extended browser/devices, older OS version
+Niche screen resolution &amp; orientation handlin</t>
+  </si>
+  <si>
+    <t>User experience / Usability Testing</t>
+  </si>
+  <si>
+    <t>Exploratory sessions for intuitiveness (?)
+A/B test validation if enable (?)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P0 - High priority</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(App up? Core logic ok?)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P1 - Medium Priority</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(Error handled? Works everywhere?)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P2: Extended Quality Non-functional</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(Fast, secure, accessible, beautiful?)</t>
+    </r>
+  </si>
+  <si>
+    <t>Core API validation</t>
+  </si>
+  <si>
+    <t>POST 200 ok
+correct JSON</t>
+  </si>
+  <si>
+    <t>Input Validation
+(functional)</t>
+  </si>
+  <si>
+    <t>Negative Testing</t>
+  </si>
+  <si>
+    <t>Invalid input
+Invalid data return 400</t>
+  </si>
+  <si>
+    <t>Visual &amp; UI consistency
+UI/UX polish</t>
+  </si>
+  <si>
+    <t>Icon alignment, tooltips
+Visual regression on components
+Dark mode, RTL layouts, theming</t>
+  </si>
+  <si>
+    <t>Login/Authen flows impacted by the feature</t>
+  </si>
+  <si>
+    <t>Boundary values (max/min)
+Missing mandatory fields / Empty fields
+Special characters
+Session timeout</t>
+  </si>
+  <si>
+    <t>Data Integrity</t>
+  </si>
+  <si>
+    <t>Primary User Journey
+Must work business rule</t>
+  </si>
+  <si>
+    <t>UI behavior</t>
+  </si>
+  <si>
+    <t>Filtering &amp; sorting (default &amp; non-default)</t>
+  </si>
+  <si>
+    <t>Authz on endpoints (403)
+Token</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test priority</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> defines the execution order and focus based on business impact, user risk, and system stability. It ensures that the most critical checks (those that confirm basic functionality and prevent showstoppers) run first.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Main features (Positive Path)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Main Flow</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CRUD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with valid data</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>State Transition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>states transitions / events</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>flow chart</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Experience-Based
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Based on tester skills &amp; domain knowledge</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Error Guessing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Use common failures 
+- Input (Missing parameter)
+- Ouput (wrong format, wrong result)
+- Nulls
+- encoding
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exploratory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+When you need fast learning in a short time. 
+There is a time pressure. Guided by a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">charter </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(goal, scope, risk, constraints)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Test tours</t>
+  </si>
+  <si>
+    <t>Session-Based Test Management ()</t>
+  </si>
+  <si>
+    <t>Pair /Mob Testing</t>
+  </si>
+  <si>
+    <t>Dimension</t>
+  </si>
+  <si>
+    <t>Waterfall</t>
+  </si>
+  <si>
+    <t>V-Model</t>
+  </si>
+  <si>
+    <t>Iterative/Incremental</t>
+  </si>
+  <si>
+    <t>Agile / Scrum</t>
+  </si>
+  <si>
+    <t>DevOps / CI-CD</t>
+  </si>
+  <si>
+    <t>When testing happens</t>
+  </si>
+  <si>
+    <t>Test design</t>
+  </si>
+  <si>
+    <t>Evolving test design per increment</t>
+  </si>
+  <si>
+    <r>
+      <t>Risk-based</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exploratory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + lightweight cases</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pipelines</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> define checks; contracts, monitors</t>
+    </r>
+  </si>
+  <si>
+    <t>Shift-left</t>
+  </si>
+  <si>
+    <t>Low–medium</t>
+  </si>
+  <si>
+    <t>High (reviews/analysis)</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High (ATDD/BDD, pairing)</t>
+  </si>
+  <si>
+    <t>Very high (pre-merge gates)</t>
+  </si>
+  <si>
+    <t>Shift-right</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium (feature flags, canaries)</t>
+  </si>
+  <si>
+    <t>High (synthetics, SLOs, chaos)</t>
+  </si>
+  <si>
+    <t>Automation focus</t>
+  </si>
+  <si>
+    <t>Late UI/system/regression</t>
+  </si>
+  <si>
+    <t>Unit + system to mirror “V”</t>
+  </si>
+  <si>
+    <t>Unit/integration grow over time</t>
+  </si>
+  <si>
+    <r>
+      <t>Test pyramid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (unit/component &gt; API &gt; few E2E)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Continuous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> unit/integration/contract; deploy gates</t>
+    </r>
+  </si>
+  <si>
+    <t>Environments</t>
+  </si>
+  <si>
+    <t>Dedicated test/UAT; infrequent refresh</t>
+  </si>
+  <si>
+    <t>Controlled, validated envs</t>
+  </si>
+  <si>
+    <t>Incremental envs</t>
+  </si>
+  <si>
+    <t>Ephemeral envs per branch; stubs/mocks</t>
+  </si>
+  <si>
+    <r>
+      <t>Ephemeral/On-demand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, prod parity; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>feature flags</t>
+    </r>
+  </si>
+  <si>
+    <t>Integration strategy</t>
+  </si>
+  <si>
+    <t>Big-bang</t>
+  </si>
+  <si>
+    <t>Staged by level</t>
+  </si>
+  <si>
+    <t>By increment</t>
+  </si>
+  <si>
+    <r>
+      <t>CI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> each commit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Trunk-based</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contract tests</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>canary</t>
+    </r>
+  </si>
+  <si>
+    <t>Docs &amp; traceability</t>
+  </si>
+  <si>
+    <t>Heavy; formal approvals</t>
+  </si>
+  <si>
+    <r>
+      <t>Strict traceability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> req→tests</t>
+    </r>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Lean (AC, BDD scenarios)</t>
+  </si>
+  <si>
+    <t>Pipelines-as-evidence; living docs</t>
+  </si>
+  <si>
+    <t>Defect handling</t>
+  </si>
+  <si>
+    <t>Central triage; longer cycles</t>
+  </si>
+  <si>
+    <t>Severity gates tied to “V” layer</t>
+  </si>
+  <si>
+    <t>Incremental triage</t>
+  </si>
+  <si>
+    <t>Daily triage</t>
+  </si>
+  <si>
+    <r>
+      <t>Automated rollback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; observability-driven triage</t>
+    </r>
+  </si>
+  <si>
+    <t>Best fit</t>
+  </si>
+  <si>
+    <t>Stable reqs; low change</t>
+  </si>
+  <si>
+    <t>Safety/regulated domains</t>
+  </si>
+  <si>
+    <t>Complex systems maturing</t>
+  </si>
+  <si>
+    <t>Product discovery, rapid change</t>
+  </si>
+  <si>
+    <t>SaaS/Cloud at scale, rapid delivery</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Early </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>static reviews</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; 
+formal mapping from artifacts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mostly </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>after build</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mirrors dev phase </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(req↔UAT, 
+design↔system, 
+unit↔impl)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Each increment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tested</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Every sprint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; continuous</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Every commit/merge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; 
+in prod too</t>
+    </r>
+  </si>
+  <si>
+    <t>Full test plan early; 
+heavy scripted</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Checklist-based</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Write, implement, run from a checklist</t>
+    </r>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,16 +2329,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -793,11 +2406,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -808,7 +2456,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -831,12 +2478,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -845,9 +2486,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -864,6 +2502,111 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,6 +2623,276 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2065019</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1839729</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1607820" y="297180"/>
+          <a:ext cx="1943099" cy="1725429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2471957</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1798320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="SDLC - V Model - Notepub"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3710941" y="304800"/>
+          <a:ext cx="2357656" cy="1676400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19593</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>281940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2362200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1593800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Iterative and incremental development - Wikipedia"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6161313" y="464820"/>
+          <a:ext cx="2342607" cy="1311860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>167869</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2217420</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1638299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="The Agile Software Development Life Cycle | Wrike Agile Guide"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="8164" r="6998"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8511540" y="350749"/>
+          <a:ext cx="2217420" cy="1470430"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2209800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>96201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1699259</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="DevOps: the pillars to accelerate the SDLC | Mia-Platform"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a14:imgLayer r:embed="rId6">
+                  <a14:imgEffect>
+                    <a14:backgroundRemoval t="10000" b="90000" l="8021" r="93281"/>
+                  </a14:imgEffect>
+                </a14:imgLayer>
+              </a14:imgProps>
+            </a:ext>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10721340" y="279081"/>
+          <a:ext cx="2849880" cy="1603058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1148,7 +3161,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="E4" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,171 +3176,171 @@
     <col min="8" max="8" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="26" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:8" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1344,6 +3357,257 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="3" max="3" width="37.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" customWidth="1"/>
+    <col min="6" max="6" width="37.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1352,231 +3616,560 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="35" style="20" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="35" style="16" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="16" customWidth="1"/>
     <col min="4" max="4" width="17.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" style="19" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="6" width="30" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="25.77734375" style="23" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="42" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="43" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="41" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="166.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="44"/>
+      <c r="B6" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="44"/>
+      <c r="B7" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C8" s="54" t="s">
         <v>92</v>
       </c>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="36"/>
+      <c r="B3" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="36"/>
+      <c r="B4" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="36"/>
+      <c r="B5" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>95</v>
+      <c r="A6" s="36"/>
+      <c r="B6" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>56</v>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="36"/>
+      <c r="B8" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="29"/>
+      <c r="B10" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="29"/>
+      <c r="B11" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="29"/>
+      <c r="B12" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
+      <c r="B14" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="29"/>
+      <c r="B15" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="32"/>
+    </row>
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="29"/>
+      <c r="B16" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="29"/>
+      <c r="B17" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="33"/>
+      <c r="B19" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
+      <c r="B20" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="33"/>
+      <c r="B21" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="33"/>
+      <c r="B22" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="33"/>
+      <c r="B23" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="33"/>
+      <c r="B24" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 7 testing principles
</commit_message>
<xml_diff>
--- a/Others/Testing levels comparison.xlsx
+++ b/Others/Testing levels comparison.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Levels" sheetId="1" r:id="rId1"/>
     <sheet name="SDLC" sheetId="5" r:id="rId2"/>
-    <sheet name="Planning" sheetId="2" r:id="rId3"/>
-    <sheet name="Static vs Dynamic" sheetId="3" r:id="rId4"/>
-    <sheet name="Test order" sheetId="4" r:id="rId5"/>
+    <sheet name="7 principles" sheetId="6" r:id="rId3"/>
+    <sheet name="Planning" sheetId="2" r:id="rId4"/>
+    <sheet name="Static vs Dynamic" sheetId="3" r:id="rId5"/>
+    <sheet name="Test order" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="247">
   <si>
     <t>Test Level</t>
   </si>
@@ -2286,6 +2287,220 @@
   </si>
   <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Agile = Iterative + incremental
+But with a time frame </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(sprint)</t>
+    </r>
+  </si>
+  <si>
+    <t>Principle</t>
+  </si>
+  <si>
+    <t>Explain</t>
+  </si>
+  <si>
+    <t>Testing shows the presence of defects, not their absence</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tests can reveal problems, but can't prove there are none.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-&gt; Stop chasing "Zero bug". Aim for risk deduction &amp; confidence</t>
+    </r>
+  </si>
+  <si>
+    <t>Exhaustive testng is impossible</t>
+  </si>
+  <si>
+    <t>Early testing saves time and money</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Find issues when they're cheap - during requirements, design and implement. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-&gt; Shift left</t>
+    </r>
+  </si>
+  <si>
+    <t>Defects cluster together</t>
+  </si>
+  <si>
+    <t>Tests wear out</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repeating the same test will become ineffective</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-&gt; Update test data &amp; scenarios</t>
+    </r>
+  </si>
+  <si>
+    <t>Testing is context dependent</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Banking is diferent with Health and Gaming. 
+-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Testing is done differently in diff context.</t>
+    </r>
+  </si>
+  <si>
+    <t>Absence-of-errors fallacy</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A product is bug-free but doesn't meet requirement still fails.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-&gt; Priority the purpose of the product, not the bug hunting. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Can't test every input, path,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> locale, device…
+-&gt; Apply techniques like </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">EP/BVA, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>decision tables,…</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A small number of modules tend to contain most defects. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-&gt; Focus on hotspots (complex code, heavy change, past bugs...)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2445,7 +2660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2516,97 +2731,106 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2778,15 +3002,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>167869</xdr:rowOff>
+      <xdr:rowOff>129769</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2217420</xdr:colOff>
+      <xdr:colOff>2308860</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1638299</xdr:rowOff>
+      <xdr:rowOff>1600199</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2808,7 +3032,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8511540" y="350749"/>
+          <a:off x="8602980" y="312649"/>
           <a:ext cx="2217420" cy="1470430"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3219,10 +3443,10 @@
       <c r="F2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="50" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3245,11 +3469,11 @@
       <c r="F3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
     </row>
     <row r="4" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -3261,7 +3485,7 @@
       <c r="D4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="50" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="11" t="s">
@@ -3270,10 +3494,10 @@
       <c r="G4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="26"/>
+      <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
@@ -3283,14 +3507,14 @@
       <c r="D5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="50"/>
       <c r="F5" s="11" t="s">
         <v>30</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="50" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3316,7 +3540,7 @@
       <c r="G6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="26"/>
+      <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:8" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -3340,7 +3564,7 @@
       <c r="G7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3359,9 +3583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3394,219 +3618,310 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>228</v>
       </c>
       <c r="B2" s="21"/>
+      <c r="D2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="26" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="25" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="26" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="26" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="25" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="25" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="25" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="26" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="25" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="26" t="s">
         <v>219</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" style="56" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="57" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="114" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="57" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="57" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="57" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="57" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="57" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -3755,7 +4070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -3776,29 +4091,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="36" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="37" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="35" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="19" t="s">
@@ -3809,63 +4124,63 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="35" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="43" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="44" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="166.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45" t="s">
+      <c r="A6" s="51"/>
+      <c r="B6" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="G6" s="53" t="s">
+      <c r="G6" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="46" t="s">
         <v>107</v>
       </c>
       <c r="I6" s="5"/>
@@ -3873,47 +4188,47 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
-      <c r="B7" s="45" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="G7" s="55" t="s">
+      <c r="G7" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="I7" s="49" t="s">
+      <c r="I7" s="42" t="s">
         <v>162</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="35" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="47" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="19"/>
@@ -3928,12 +4243,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3945,220 +4260,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="34" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37" t="s">
+      <c r="A3" s="52"/>
+      <c r="B3" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="33" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="33" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="33" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37" t="s">
+      <c r="A6" s="52"/>
+      <c r="B6" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="33" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="33" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="37" t="s">
+      <c r="A8" s="52"/>
+      <c r="B8" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="33" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="28" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30" t="s">
+      <c r="A10" s="54"/>
+      <c r="B10" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="29" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="54"/>
+      <c r="B11" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="29" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
-      <c r="B12" s="31" t="s">
+      <c r="A12" s="54"/>
+      <c r="B12" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="29" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30" t="s">
+      <c r="A13" s="54"/>
+      <c r="B13" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="29" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
-      <c r="B14" s="31" t="s">
+      <c r="A14" s="54"/>
+      <c r="B14" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="29" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="54"/>
+      <c r="B15" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
-      <c r="B16" s="31" t="s">
+      <c r="A16" s="54"/>
+      <c r="B16" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="29" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="29"/>
-      <c r="B17" s="31" t="s">
+      <c r="A17" s="54"/>
+      <c r="B17" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="29" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="31" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34" t="s">
+      <c r="A19" s="53"/>
+      <c r="B19" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="31" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34" t="s">
+      <c r="A20" s="53"/>
+      <c r="B20" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="31" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="53"/>
+      <c r="B21" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="31" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="33"/>
-      <c r="B22" s="34" t="s">
+      <c r="A22" s="53"/>
+      <c r="B22" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="31" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="33"/>
-      <c r="B23" s="34" t="s">
+      <c r="A23" s="53"/>
+      <c r="B23" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="31" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="33"/>
-      <c r="B24" s="34" t="s">
+      <c r="A24" s="53"/>
+      <c r="B24" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="31" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>